<commit_message>
Added last digit percentage column and snapshots
</commit_message>
<xml_diff>
--- a/Benfords_law_covid_cases.xlsx
+++ b/Benfords_law_covid_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Benfords law\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80AF6ABF-9B7F-44B9-BCC4-E7AB4E9D213B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D69337-27A0-4C1B-924D-F052435786FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="16836" windowHeight="8964"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benfords_law_covid_cases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>DIGIT</t>
   </si>
@@ -28,16 +28,19 @@
     <t>num_cases</t>
   </si>
   <si>
-    <t>Covid_dataset_percentage</t>
+    <t>Benfords_law_percentage</t>
   </si>
   <si>
-    <t>Benfords_law_percentage</t>
+    <t>Covid_dataset_last_digit_percentage</t>
+  </si>
+  <si>
+    <t>Covid_dataset_first_digit_percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -871,14 +874,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -886,13 +898,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -905,8 +920,11 @@
       <c r="D2">
         <v>30.1</v>
       </c>
+      <c r="E2">
+        <v>13.4093</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -919,8 +937,11 @@
       <c r="D3">
         <v>17.600000000000001</v>
       </c>
+      <c r="E3">
+        <v>12.118</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -933,8 +954,11 @@
       <c r="D4">
         <v>12.5</v>
       </c>
+      <c r="E4">
+        <v>11.683299999999999</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -947,8 +971,11 @@
       <c r="D5">
         <v>9.6999999999999993</v>
       </c>
+      <c r="E5">
+        <v>10.9939</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -961,8 +988,11 @@
       <c r="D6">
         <v>7.9</v>
       </c>
+      <c r="E6">
+        <v>10.724</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -975,8 +1005,11 @@
       <c r="D7">
         <v>6.7</v>
       </c>
+      <c r="E7">
+        <v>10.507</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -989,8 +1022,11 @@
       <c r="D8">
         <v>5.8</v>
       </c>
+      <c r="E8">
+        <v>10.299899999999999</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1003,8 +1039,11 @@
       <c r="D9">
         <v>5.0999999999999996</v>
       </c>
+      <c r="E9">
+        <v>10.1943</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1016,6 +1055,9 @@
       </c>
       <c r="D10">
         <v>4.5999999999999996</v>
+      </c>
+      <c r="E10">
+        <v>10.070499999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>